<commit_message>
BACKEND-2 tfgs asig masivos dni alum
</commit_message>
<xml_diff>
--- a/apps/upload_files/tests/test_upload_file_tfgs/ListaTFGs_preasignados.xlsx
+++ b/apps/upload_files/tests/test_upload_file_tfgs/ListaTFGs_preasignados.xlsx
@@ -98,7 +98,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>tonima@correo.ugr.es</t>
+    <t>75169052S</t>
   </si>
   <si>
     <r>
@@ -3780,7 +3780,7 @@
   <dimension ref="1:9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6096,13 +6096,12 @@
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="jorgecasillas@ugr.es"/>
     <hyperlink ref="C5" r:id="rId2" display="miguelgarcia@ugr.es"/>
-    <hyperlink ref="G5" r:id="rId3" display="tonima@correo.ugr.es"/>
-    <hyperlink ref="H6" r:id="rId4" display="fewugb@correo.ugr.es"/>
-    <hyperlink ref="B7" r:id="rId5" display="juanmanuelfernandez@ugr.es"/>
-    <hyperlink ref="B8" r:id="rId6" display="eugenioaguirre@ugr.es"/>
-    <hyperlink ref="C8" r:id="rId7" display="miguelgarcia@ugr.es"/>
-    <hyperlink ref="H8" r:id="rId8" display="w4rwe@correo.ugr.es"/>
-    <hyperlink ref="B9" r:id="rId9" display="franciscoherrera@ugr.es"/>
+    <hyperlink ref="H6" r:id="rId3" display="fewugb@correo.ugr.es"/>
+    <hyperlink ref="B7" r:id="rId4" display="juanmanuelfernandez@ugr.es"/>
+    <hyperlink ref="B8" r:id="rId5" display="eugenioaguirre@ugr.es"/>
+    <hyperlink ref="C8" r:id="rId6" display="miguelgarcia@ugr.es"/>
+    <hyperlink ref="H8" r:id="rId7" display="w4rwe@correo.ugr.es"/>
+    <hyperlink ref="B9" r:id="rId8" display="franciscoherrera@ugr.es"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.0784722222222222" right="0.0784722222222222" top="0.493055555555556" bottom="0.493055555555556" header="0.354166666666667" footer="0.354166666666667"/>
@@ -6122,7 +6121,7 @@
   <dimension ref="A1:IW173"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="C5 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="9.95"/>
@@ -23144,7 +23143,7 @@
   <dimension ref="1:151"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
@@ -37860,7 +37859,7 @@
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -39199,7 +39198,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>

</xml_diff>